<commit_message>
Few file reference changes
</commit_message>
<xml_diff>
--- a/FinalProject/Client_Data.xlsx
+++ b/FinalProject/Client_Data.xlsx
@@ -19,32 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
-  <si>
-    <t>Swapnil</t>
-  </si>
-  <si>
-    <t>Desai</t>
-  </si>
-  <si>
-    <t>Bardoli</t>
-  </si>
-  <si>
-    <t>Student</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Checking</t>
   </si>
   <si>
-    <t>Dhruv</t>
-  </si>
-  <si>
-    <t>Sherathiya</t>
-  </si>
-  <si>
-    <t>Junagadh</t>
-  </si>
-  <si>
     <t>Savings</t>
   </si>
   <si>
@@ -70,6 +49,30 @@
   </si>
   <si>
     <t>amount</t>
+  </si>
+  <si>
+    <t>Lockwood</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Tyler</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>Wisconsin</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Analyst</t>
   </si>
 </sst>
 </file>
@@ -395,7 +398,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,28 +408,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -434,22 +437,22 @@
         <v>1503541429</v>
       </c>
       <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1">
+        <v>36089</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
         <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1">
-        <v>35717</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
-        <v>4</v>
       </c>
       <c r="H2">
         <v>2000000</v>
@@ -460,22 +463,22 @@
         <v>1387341967</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2">
-        <v>35939</v>
+        <v>33219</v>
       </c>
       <c r="F3" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <v>100000</v>

</xml_diff>